<commit_message>
Working on Factor Analysis and LCA
Currently trying in both stata and R. Created new scripts/dofiles for both
</commit_message>
<xml_diff>
--- a/R/Crosswave-Variable-List.xlsx
+++ b/R/Crosswave-Variable-List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9E2518-AAEF-43D6-B65A-DA734B0B5718}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1336C74-24F4-4179-A3B6-C3E407BF7D7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38460" yWindow="7335" windowWidth="19920" windowHeight="7425" xr2:uid="{EDEBDEAC-AFAE-43FD-9A26-9B7F903D004C}"/>
   </bookViews>
@@ -5378,7 +5378,7 @@
   <dimension ref="A1:L336"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>